<commit_message>
Adds styling and AI notes for Rookie Free Agents
</commit_message>
<xml_diff>
--- a/python_analysis/data/common/RSP_Rookies.xlsx
+++ b/python_analysis/data/common/RSP_Rookies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/common/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/volatile/python_analysis/data/common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{80AFF0B4-8318-5B46-9F51-C5E54E028385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D809908-1E06-438E-9F00-18100E73A9DE}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{80AFF0B4-8318-5B46-9F51-C5E54E028385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E40CF8-DFDE-47A9-B703-79CE089BE237}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15460" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1485,10 +1485,6 @@
     <t>Jake Plummer / J.J. McCarthy (High End / Stylistic) – Drew Lock / Zach Wilson (Low End / Volatility)</t>
   </si>
   <si>
-    <t>Official Spectrum: Josh Allen / Andrew Luck (High End / Toolsy Potential) – Tim Tebow / Bryce Petty (Low End / Limited Passer)
-Elaborated Comparison: The "Frankenstein" analogy (Allen + Tebow DNA) producing either Luck (refined) or Howard ("Young Frankenstein" - raw potential) highlights his profile as having high-upside physical tools but significant questions about processing and passing refinement, leading to a wide range of potential outcomes.</t>
-  </si>
-  <si>
     <t>Official Spectrum: Brock Purdy (High End - efficient system QB) – C.J. Beathard (Low End - career backup/spot starter)</t>
   </si>
   <si>
@@ -1958,6 +1954,10 @@
 Mention: Stephen Davis: An aspirational comparison highlighting elite power potential if Mafah fully refines that aspect.
 Fantasy Outlook (.5 PPR - As of April 28, 2025):
 Now on an NFL roster, Phil Mafah profiles primarily as an early-down and short-yardage/goal-line specialist early in his career. His size, power, and rushing acumen provide a solid foundation for fantasy value through carries and touchdowns. However, his .5 PPR upside is significantly limited by major deficiencies in both pass protection and receiving technique. Until he makes substantial improvements in these areas, he is unlikely to command significant passing-down work or reception volume. Expect him to function within a committee, offering RB2/Flex value based on rushing workload and TD opportunities, rather than as a high-volume PPR contributor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Official Spectrum: Josh Allen / Andrew Luck (High End / Toolsy Potential) – Tim Tebow / Bryce Petty (Low End / Limited Passer)
+</t>
   </si>
 </sst>
 </file>
@@ -2013,10 +2013,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2339,8 +2335,8 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2933,7 +2929,7 @@
         <v>222</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3017,7 +3013,7 @@
         <v>154</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3275,7 +3271,7 @@
         <v>154</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3826,7 +3822,7 @@
         <v>222</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3846,7 +3842,7 @@
         <v>62</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>226</v>
+        <v>275</v>
       </c>
       <c r="G52">
         <v>76.260000000000005</v>
@@ -3855,7 +3851,7 @@
         <v>154</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
@@ -3875,7 +3871,7 @@
         <v>113</v>
       </c>
       <c r="F53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G53">
         <v>74</v>
@@ -3884,12 +3880,12 @@
         <v>152</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3898,10 +3894,10 @@
         <v>27</v>
       </c>
       <c r="E54" t="s">
+        <v>245</v>
+      </c>
+      <c r="F54" t="s">
         <v>246</v>
-      </c>
-      <c r="F54" t="s">
-        <v>247</v>
       </c>
       <c r="G54">
         <v>82.4</v>
@@ -3910,12 +3906,12 @@
         <v>135</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -3927,7 +3923,7 @@
         <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G55">
         <v>81.900000000000006</v>
@@ -3936,12 +3932,12 @@
         <v>135</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -3950,10 +3946,10 @@
         <v>58</v>
       </c>
       <c r="E56" t="s">
+        <v>248</v>
+      </c>
+      <c r="F56" t="s">
         <v>249</v>
-      </c>
-      <c r="F56" t="s">
-        <v>250</v>
       </c>
       <c r="G56">
         <v>73.8</v>
@@ -3962,12 +3958,12 @@
         <v>152</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -3979,7 +3975,7 @@
         <v>91</v>
       </c>
       <c r="F57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G57">
         <v>83</v>
@@ -3988,12 +3984,12 @@
         <v>135</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
@@ -4005,7 +4001,7 @@
         <v>77</v>
       </c>
       <c r="F58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G58">
         <v>77.400000000000006</v>
@@ -4014,12 +4010,12 @@
         <v>154</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -4031,7 +4027,7 @@
         <v>111</v>
       </c>
       <c r="F59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G59">
         <v>73.8</v>
@@ -4040,12 +4036,12 @@
         <v>152</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -4057,7 +4053,7 @@
         <v>131</v>
       </c>
       <c r="F60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G60">
         <v>75.099999999999994</v>
@@ -4066,12 +4062,12 @@
         <v>135</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
@@ -4083,7 +4079,7 @@
         <v>113</v>
       </c>
       <c r="F61" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G61">
         <v>81.5</v>
@@ -4092,12 +4088,12 @@
         <v>135</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
@@ -4106,10 +4102,10 @@
         <v>21</v>
       </c>
       <c r="E62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G62">
         <v>80.7</v>
@@ -4118,12 +4114,12 @@
         <v>135</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
@@ -4135,7 +4131,7 @@
         <v>136</v>
       </c>
       <c r="F63" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G63">
         <v>83.4</v>
@@ -4144,12 +4140,12 @@
         <v>135</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
@@ -4158,10 +4154,10 @@
         <v>14</v>
       </c>
       <c r="E64" t="s">
+        <v>261</v>
+      </c>
+      <c r="F64" t="s">
         <v>262</v>
-      </c>
-      <c r="F64" t="s">
-        <v>263</v>
       </c>
       <c r="G64">
         <v>83.4</v>
@@ -4170,12 +4166,12 @@
         <v>135</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
@@ -4184,19 +4180,19 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
+        <v>258</v>
+      </c>
+      <c r="F65" t="s">
         <v>259</v>
-      </c>
-      <c r="F65" t="s">
-        <v>260</v>
       </c>
       <c r="G65">
         <v>82.3</v>
       </c>
       <c r="H65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>